<commit_message>
update guide and readme
</commit_message>
<xml_diff>
--- a/sample/exp0_vs_exp1/death/hr_main.xlsx
+++ b/sample/exp0_vs_exp1/death/hr_main.xlsx
@@ -407,10 +407,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>0.502289043020301</v>
+        <v>0.5022890430203012</v>
       </c>
       <c r="B3">
-        <v>0.09378184837264687</v>
+        <v>0.09378184837264696</v>
       </c>
       <c r="C3">
         <v>2.690225103430952</v>

</xml_diff>